<commit_message>
feat: 자재 LOT 조회 type 파라미터 추가 및 Slurry LOT 목록 API 추가
</commit_message>
<xml_diff>
--- a/data/templates/worklog/03.Coating.xlsx
+++ b/data/templates/worklog/03.Coating.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\eurocell-mes-be\data\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\eurocell-mes-be\data\templates\worklog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172C3EBD-6743-4145-AD85-8E5D9EC6407D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCF0BC9-48ED-4691-AB8D-32AAF10D2A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="0" windowWidth="19140" windowHeight="15210" xr2:uid="{1FFCD294-0548-4598-B62F-70ED7559ADF2}"/>
+    <workbookView xWindow="1590" yWindow="930" windowWidth="18735" windowHeight="13965" xr2:uid="{1FFCD294-0548-4598-B62F-70ED7559ADF2}"/>
   </bookViews>
   <sheets>
     <sheet name="원본" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
   <si>
     <t>코팅 작업 일지</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -443,6 +443,10 @@
   </si>
   <si>
     <t>무지부</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slurry</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -963,6 +967,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -972,6 +985,147 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -998,156 +1152,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1490,8 +1494,8 @@
   </sheetPr>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1500,17 +1504,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
       <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1522,288 +1526,290 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="73"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="73"/>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="14"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="17"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="70" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="70"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="70" t="s">
+      <c r="F7" s="13"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="70"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="70" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="70"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="70" t="s">
+      <c r="F8" s="13"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="70"/>
-      <c r="K8" s="72" t="s">
+      <c r="J8" s="13"/>
+      <c r="K8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="72"/>
+      <c r="L8" s="12"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="14"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="17"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="70" t="s">
+      <c r="A10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="71" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71" t="s">
+      <c r="D10" s="21"/>
+      <c r="E10" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="71"/>
-      <c r="G10" s="70" t="s">
+      <c r="F10" s="21"/>
+      <c r="G10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="70"/>
-      <c r="I10" s="71" t="s">
+      <c r="H10" s="13"/>
+      <c r="I10" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="71"/>
-      <c r="K10" s="70" t="s">
+      <c r="J10" s="21"/>
+      <c r="K10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="70"/>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="69" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="70" t="s">
+      <c r="A12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="71" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71" t="s">
+      <c r="D12" s="21"/>
+      <c r="E12" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="71"/>
-      <c r="G12" s="70" t="s">
+      <c r="F12" s="21"/>
+      <c r="G12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="70"/>
-      <c r="I12" s="71" t="s">
+      <c r="H12" s="13"/>
+      <c r="I12" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="71"/>
-      <c r="K12" s="70" t="s">
+      <c r="J12" s="21"/>
+      <c r="K12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="70"/>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="69"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="69"/>
+      <c r="A13" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
     </row>
     <row r="14" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="66"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="66"/>
-      <c r="L14" s="67"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="24"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="60"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="11" t="s">
         <v>62</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="57" t="s">
+      <c r="G15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="58"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="61"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="31"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="62" t="s">
+      <c r="B16" s="33"/>
+      <c r="C16" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="63"/>
+      <c r="D16" s="35"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
-      <c r="G16" s="62" t="s">
+      <c r="G16" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="63"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="62" t="s">
+      <c r="H16" s="35"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="K16" s="63"/>
-      <c r="L16" s="64"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="36"/>
     </row>
     <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="49" t="s">
+      <c r="B17" s="33"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="49"/>
+      <c r="F17" s="39"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1812,14 +1818,14 @@
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -1828,60 +1834,60 @@
       <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="60"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="11" t="s">
         <v>62</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="57" t="s">
+      <c r="G19" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="58"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="61"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="31"/>
     </row>
     <row r="20" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="62" t="s">
+      <c r="B20" s="33"/>
+      <c r="C20" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="63"/>
+      <c r="D20" s="35"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="62" t="s">
+      <c r="G20" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="63"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="62" t="s">
+      <c r="H20" s="35"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="K20" s="63"/>
-      <c r="L20" s="64"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="36"/>
     </row>
     <row r="21" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="46"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="49" t="s">
+      <c r="B21" s="33"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="49"/>
+      <c r="F21" s="39"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1890,14 +1896,14 @@
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -1906,60 +1912,60 @@
       <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="55" t="s">
+      <c r="A23" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="56"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="60"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
       <c r="E23" s="11" t="s">
         <v>62</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="57" t="s">
+      <c r="G23" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="58"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="61"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="31"/>
     </row>
     <row r="24" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="46"/>
-      <c r="C24" s="62" t="s">
+      <c r="B24" s="33"/>
+      <c r="C24" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="63"/>
+      <c r="D24" s="35"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
-      <c r="G24" s="62" t="s">
+      <c r="G24" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="63"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="62" t="s">
+      <c r="H24" s="35"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="63"/>
-      <c r="L24" s="64"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="36"/>
     </row>
     <row r="25" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="49" t="s">
+      <c r="B25" s="33"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="49"/>
+      <c r="F25" s="39"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1968,14 +1974,14 @@
       <c r="L25" s="3"/>
     </row>
     <row r="26" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="50" t="s">
+      <c r="A26" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="51"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
@@ -1984,60 +1990,60 @@
       <c r="L26" s="9"/>
     </row>
     <row r="27" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="56"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="60"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="11" t="s">
         <v>62</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G27" s="57" t="s">
+      <c r="G27" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="58"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="59"/>
-      <c r="K27" s="60"/>
-      <c r="L27" s="61"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="31"/>
     </row>
     <row r="28" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="62" t="s">
+      <c r="B28" s="33"/>
+      <c r="C28" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="63"/>
+      <c r="D28" s="35"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
-      <c r="G28" s="62" t="s">
+      <c r="G28" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="63"/>
-      <c r="I28" s="46"/>
-      <c r="J28" s="62" t="s">
+      <c r="H28" s="35"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="K28" s="63"/>
-      <c r="L28" s="64"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="36"/>
     </row>
     <row r="29" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="49" t="s">
+      <c r="B29" s="33"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="F29" s="49"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -2046,14 +2052,14 @@
       <c r="L29" s="3"/>
     </row>
     <row r="30" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="50" t="s">
+      <c r="A30" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
@@ -2062,357 +2068,488 @@
       <c r="L30" s="5"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="40"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="47"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="42"/>
-      <c r="C32" s="43" t="s">
+      <c r="B32" s="49"/>
+      <c r="C32" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="44"/>
-      <c r="E32" s="43" t="s">
+      <c r="D32" s="51"/>
+      <c r="E32" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="F32" s="44"/>
-      <c r="G32" s="43" t="s">
+      <c r="F32" s="51"/>
+      <c r="G32" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="H32" s="44"/>
-      <c r="I32" s="43" t="s">
+      <c r="H32" s="51"/>
+      <c r="I32" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="J32" s="44"/>
-      <c r="K32" s="43" t="s">
+      <c r="J32" s="51"/>
+      <c r="K32" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="L32" s="44"/>
+      <c r="L32" s="51"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="35" t="s">
+      <c r="B33" s="55"/>
+      <c r="C33" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="36"/>
+      <c r="D33" s="59"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="35"/>
-      <c r="L33" s="36"/>
+      <c r="I33" s="58"/>
+      <c r="J33" s="59"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="59"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="33"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="35" t="s">
+      <c r="A34" s="56"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="36"/>
+      <c r="D34" s="59"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="35"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="35"/>
-      <c r="L34" s="36"/>
+      <c r="I34" s="58"/>
+      <c r="J34" s="59"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="59"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="33"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="31" t="s">
+      <c r="A35" s="56"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="32"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="32"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="60"/>
+      <c r="L35" s="55"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="28"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="27" t="s">
+      <c r="B36" s="53"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="28"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="27" t="s">
+      <c r="F36" s="53"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="J36" s="28"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="32"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="54"/>
+      <c r="L36" s="55"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="28"/>
-      <c r="C37" s="25" t="s">
+      <c r="B37" s="53"/>
+      <c r="C37" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25" t="s">
+      <c r="D37" s="61"/>
+      <c r="E37" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25" t="s">
+      <c r="F37" s="61"/>
+      <c r="G37" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25" t="s">
+      <c r="H37" s="61"/>
+      <c r="I37" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="J37" s="25" t="s">
+      <c r="J37" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="K37" s="25"/>
+      <c r="K37" s="61"/>
       <c r="L37" s="6"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="29"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25" t="s">
+      <c r="A38" s="63"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="61"/>
+      <c r="G38" s="61"/>
+      <c r="H38" s="61"/>
+      <c r="I38" s="61"/>
+      <c r="J38" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="K38" s="25"/>
+      <c r="K38" s="61"/>
       <c r="L38" s="6"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="13"/>
-      <c r="L39" s="14"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="17"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="26" t="s">
+      <c r="A40" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="24" t="s">
+      <c r="B40" s="18"/>
+      <c r="C40" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="D40" s="25"/>
-      <c r="E40" s="26" t="s">
+      <c r="D40" s="61"/>
+      <c r="E40" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F40" s="26"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="26" t="s">
+      <c r="F40" s="18"/>
+      <c r="G40" s="61"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="J40" s="26"/>
-      <c r="K40" s="24" t="s">
+      <c r="J40" s="18"/>
+      <c r="K40" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="L40" s="25"/>
+      <c r="L40" s="61"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="14"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="17"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="26" t="s">
+      <c r="A42" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="26"/>
-      <c r="C42" s="25" t="s">
+      <c r="B42" s="18"/>
+      <c r="C42" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="25"/>
-      <c r="E42" s="26" t="s">
+      <c r="D42" s="61"/>
+      <c r="E42" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F42" s="26"/>
-      <c r="G42" s="25" t="s">
+      <c r="F42" s="18"/>
+      <c r="G42" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="H42" s="25"/>
-      <c r="I42" s="26" t="s">
+      <c r="H42" s="61"/>
+      <c r="I42" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="J42" s="26"/>
-      <c r="K42" s="25" t="s">
+      <c r="J42" s="18"/>
+      <c r="K42" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="L42" s="25"/>
+      <c r="L42" s="61"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="13"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="14"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="17"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="15"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="16"/>
-      <c r="L44" s="17"/>
+      <c r="A44" s="65"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="66"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="66"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="66"/>
+      <c r="H44" s="66"/>
+      <c r="I44" s="66"/>
+      <c r="J44" s="66"/>
+      <c r="K44" s="66"/>
+      <c r="L44" s="67"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="18"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="20"/>
+      <c r="A45" s="68"/>
+      <c r="B45" s="69"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="69"/>
+      <c r="G45" s="69"/>
+      <c r="H45" s="69"/>
+      <c r="I45" s="69"/>
+      <c r="J45" s="69"/>
+      <c r="K45" s="69"/>
+      <c r="L45" s="70"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="18"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="20"/>
+      <c r="A46" s="68"/>
+      <c r="B46" s="69"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="69"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="69"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="69"/>
+      <c r="I46" s="69"/>
+      <c r="J46" s="69"/>
+      <c r="K46" s="69"/>
+      <c r="L46" s="70"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="18"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="19"/>
-      <c r="I47" s="19"/>
-      <c r="J47" s="19"/>
-      <c r="K47" s="19"/>
-      <c r="L47" s="20"/>
+      <c r="A47" s="68"/>
+      <c r="B47" s="69"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="69"/>
+      <c r="I47" s="69"/>
+      <c r="J47" s="69"/>
+      <c r="K47" s="69"/>
+      <c r="L47" s="70"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="18"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="19"/>
-      <c r="K48" s="19"/>
-      <c r="L48" s="20"/>
+      <c r="A48" s="68"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="69"/>
+      <c r="F48" s="69"/>
+      <c r="G48" s="69"/>
+      <c r="H48" s="69"/>
+      <c r="I48" s="69"/>
+      <c r="J48" s="69"/>
+      <c r="K48" s="69"/>
+      <c r="L48" s="70"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="18"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19"/>
-      <c r="I49" s="19"/>
-      <c r="J49" s="19"/>
-      <c r="K49" s="19"/>
-      <c r="L49" s="20"/>
+      <c r="A49" s="68"/>
+      <c r="B49" s="69"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="69"/>
+      <c r="F49" s="69"/>
+      <c r="G49" s="69"/>
+      <c r="H49" s="69"/>
+      <c r="I49" s="69"/>
+      <c r="J49" s="69"/>
+      <c r="K49" s="69"/>
+      <c r="L49" s="70"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="21"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="23"/>
+      <c r="A50" s="71"/>
+      <c r="B50" s="72"/>
+      <c r="C50" s="72"/>
+      <c r="D50" s="72"/>
+      <c r="E50" s="72"/>
+      <c r="F50" s="72"/>
+      <c r="G50" s="72"/>
+      <c r="H50" s="72"/>
+      <c r="I50" s="72"/>
+      <c r="J50" s="72"/>
+      <c r="K50" s="72"/>
+      <c r="L50" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="148">
+    <mergeCell ref="A43:L43"/>
+    <mergeCell ref="A44:L50"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="A41:L41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="A33:B35"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="I35:L35"/>
+    <mergeCell ref="A31:L31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:D8"/>
@@ -2430,137 +2567,6 @@
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="A33:B35"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="I35:L35"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="A43:L43"/>
-    <mergeCell ref="A44:L50"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="A41:L41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="K42:L42"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>